<commit_message>
Added to rfid agent and added write functionality to python script for OPC stuff
</commit_message>
<xml_diff>
--- a/SimulationTagMapping.xlsx
+++ b/SimulationTagMapping.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A8993-D17A-4551-8EFD-BE3E14359905}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB3891A-0F35-43D4-85A3-9D9D8CA5950E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>RFID Agent</t>
   </si>
@@ -34,37 +34,64 @@
     <t>Conv_N053:I.Data[3].1</t>
   </si>
   <si>
-    <t>Sled_Presense_Sensor</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>If sled is present at RFID</t>
-  </si>
-  <si>
     <t>RFID_N055:I.Channel[0].TagPresent</t>
   </si>
   <si>
     <t>Tag_Presense_Sensor</t>
   </si>
   <si>
-    <t>present</t>
-  </si>
-  <si>
-    <t>not present</t>
-  </si>
-  <si>
-    <t>If part is present at RFID</t>
+    <t>Pallet_Presense_Sensor</t>
+  </si>
+  <si>
+    <t>If part is present at RFID at robot 2 stop</t>
+  </si>
+  <si>
+    <t>If pallet is present at robot 2 stop</t>
+  </si>
+  <si>
+    <t>UpdateStep_RFID3</t>
+  </si>
+  <si>
+    <t>Checks what step the RFID reader is on. If the step is 5, tag is ready for reading.</t>
+  </si>
+  <si>
+    <t>R3J_Current_Process_NO</t>
+  </si>
+  <si>
+    <t>Process # of part (should be 3 if to be processed in cell 2)</t>
+  </si>
+  <si>
+    <t>R3J_Current_Part_NO</t>
+  </si>
+  <si>
+    <t>Part number of part (Should be 2 or 3 to be processed in cell 2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -91,8 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,76 +402,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added robot agent, added to part and RFID agent, added way to lookup simulated tag from actual tag name using csv file
</commit_message>
<xml_diff>
--- a/SimulationTagMapping.xlsx
+++ b/SimulationTagMapping.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB3891A-0F35-43D4-85A3-9D9D8CA5950E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F376C9F3-062B-44D2-A62F-BBD7D9037E2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>RFID Agent</t>
   </si>
@@ -68,6 +68,21 @@
   </si>
   <si>
     <t>Part number of part (Should be 2 or 3 to be processed in cell 2)</t>
+  </si>
+  <si>
+    <t>C2RobotStop.Ext</t>
+  </si>
+  <si>
+    <t>C2RobotStopExt</t>
+  </si>
+  <si>
+    <t>Extends robot stop</t>
+  </si>
+  <si>
+    <t>C2RobotStop.Ret</t>
+  </si>
+  <si>
+    <t>C2RobotStopRet</t>
   </si>
 </sst>
 </file>
@@ -402,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,6 +502,25 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added to robot agent and RFID 3 agent. Also debugged ClientPython
</commit_message>
<xml_diff>
--- a/SimulationTagMapping.xlsx
+++ b/SimulationTagMapping.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F376C9F3-062B-44D2-A62F-BBD7D9037E2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1693FAB-BB91-4CB1-B313-09CD1E067E1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>